<commit_message>
upgrade capitalized wordcloud and other small fixes.
</commit_message>
<xml_diff>
--- a/example/titles.xlsx
+++ b/example/titles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Programming\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Programming\Python-spider-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0935ACDF-77F0-42C6-A027-5B7D0E7C985E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D8413F4-1C91-427B-BEFE-206D137D8960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11325" xr2:uid="{5A5CDDF4-5075-47D7-B4E4-8AC58C37A42D}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11325" xr2:uid="{DA9FE468-2ED0-42D0-8FAA-527D3070BDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,549 +28,731 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Progressive Feature Alignment for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Open Domain Recognition by Semantic Discrepancy Minimization.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Moving Object Detection via Contextual Information Separation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Consensus Maximization for 3D Vision Problems.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Event-Based Learning of Optical Flow, Depth, and Egomotion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Tracking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Tracking by Animation: Unsupervised Learning of Multi-Object Attentive Trackers.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Latent Filter Scaling for Multimodal Unsupervised Image-To-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Iterative Reorganization With Weak Spatial Constraints: Solving Arbitrary Jigsaw Puzzles for Unsupervised Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification by Soft Multilabel Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transferrable Prototypical Networks for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Image Generation With Semantic Parsing Transformation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Geometry-Consistent Generative Adversarial Networks for One-Sided Unsupervised Domain Mapping.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AET vs. AED: Unsupervised Representation Learning by Auto-Encoding Transformations Rather Than Data.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Towards Scene Understanding: Unsupervised Monocular Depth Estimation With Semantic-Aware Representation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DistillHash: Unsupervised Deep Hashing by Distilling Data Pairs.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Unsupervised Video Object Segmentation Through Visual Attention.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>See More, Know More: Unsupervised Video Object Segmentation With Co-Attention Siamese Networks.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Patch-Based Discriminative Feature Learning for Unsupervised Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Image Captioning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Dense Shape Correspondence.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Domain Adaptation: A Deep Max-Margin Gaussian Process Approach.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Contrastive Adaptation Network for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation for ToF Data Denoising With Adversarial Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Bilateral Cyclic Constraint and Adaptive Regularization for Unsupervised Monocular Depth Prediction.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised 3D Pose Estimation With Geometric Self-Supervision.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Embedding Learning via Invariant and Spreading Instance Feature.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Noise-Aware Unsupervised Deep Lidar-Stereo Fusion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FineGAN: Unsupervised Hierarchical Disentanglement for Fine-Grained Object Generation and Discovery.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Domain-Specific Batch Normalization for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TransGaGa: Geometry-Aware Unsupervised Image-To-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UnOS: Unified Unsupervised Optical-Flow and Stereo-Depth Estimation by Watching Videos.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GCAN: Graph Convolutional Adversarial Network for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Image Matching and Object Discovery as Optimization.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transfer Learning via Unsupervised Task Discovery for Visual Question Answering.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeepMapping: Unsupervised Map Estimation From Multiple Point Clouds.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Deep Multimodal Clustering for Unsupervised Audiovisual Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation Using Feature-Whitening and Consensus Loss.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MVTec AD - A Comprehensive Real-World Dataset for Unsupervised Anomaly Detection.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Primitive Discovery for Improved 3D Generative Modeling.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Refine and Distill: Exploiting Cycle-Inconsistency and Knowledge Distillation for Unsupervised Monocular Depth Estimation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SIGNet: Semantic Instance Aided Unsupervised 3D Geometry Perception.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Face Normalization With Extreme Pose and Expression in the Wild.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain-Specific Deblurring via Disentangled Representations.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Sliced Wasserstein Discrepancy for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Disentangling of Appearance and Geometry by Deformable Generator Network.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Modal Neural Machine Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Part-Based Disentangling of Object Shape and Appearance.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"Double-DIP": Unsupervised Image Decomposition via Coupled Deep-Image-Priors.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Action Classes With Continuous Temporal Embedding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Epipolar Flow for Stationary or Dynamic Scenes.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Quasi-Unsupervised Color Constancy.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Competitive Collaboration: Joint Unsupervised Learning of Depth, Camera Motion, Optical Flow and Motion Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Probably Symmetric Deformable 3D Objects From Images in the Wild.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Evolving Losses for Unsupervised Video Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transformation GAN for Unsupervised Image Synthesis and Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Unsupervised Hierarchical Part Decomposition of 3D Objects From a Single RGB Image.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Adaptation Learning for Hyperspectral Imagery Super-Resolution.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Creating Something From Nothing: Unsupervised Knowledge Distillation for Cross-Modal Hashing.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning for Intrinsic Image Decomposition From a Single Image.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification via Softened Similarity Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Intra-Domain Adaptation for Semantic Segmentation Through Self-Supervision.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What Can Be Transferred: Unsupervised Domain Adaptation for Endoscopic Lesions Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation With Hierarchical Gradient Synchronization.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Gum-Net: Unsupervised Geometric Matching for Fast and Accurate 3D Subtomogram Image Alignment and Averaging.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Instance Segmentation in Microscopy Images via Panoptic Domain Adaptation and Task Re-Weighting.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reliable Weighted Optimal Transport for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DUNIT: Detection-Based Unsupervised Image-to-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TransMoMo: Invariance-Driven Unsupervised Video Motion Retargeting.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Global-Local Bidirectional Reasoning for Unsupervised Representation Learning of 3D Point Clouds.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Probabilistic Structural Latent Representation for Unsupervised Embedding.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SER-FIQ: Unsupervised Estimation of Face Image Quality Based on Stochastic Embedding Robustness.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UCTGAN: Diverse Image Inpainting Based on Unsupervised Cross-Space Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Towards Unsupervised Learning of Generative Models for 3D Controllable Image Synthesis.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rotate-and-Render: Unsupervised Photorealistic Face Rotation From Single-View Images.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning by Analogy: Reliable Supervision From Transformations for Unsupervised Optical Flow Estimation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Online Deep Clustering for Unsupervised Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GraphTER: Unsupervised Learning of Graph Transformation Equivariant Representations via Auto-Encoding Node-Wise Transformations.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Representation Learning for Gaze Estimation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reusing Discriminators for Encoding: Towards Unsupervised Image-to-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Magnification of Posture Deviations Across Subjects.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation via Structurally Regularized Deep Clustering.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Stochastic Classifiers for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Intrinsic Structural Representation Points.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Shape Descriptor With Point Distribution Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning From Video With Deep Neural Embeddings.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PREDICT &amp; CLUSTER: Unsupervised Skeleton Based Action Recognition.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Model Adaptation: Unsupervised Domain Adaptation Without Source Data.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ProAlignNet: Unsupervised Learning for Progressively Aligning Noisy Contours.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Momentum Contrast for Unsupervised Visual Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Temporal Co-Attention Models for Unsupervised Video Action Localization.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Visual Grounding in Video for Unsupervised Word Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification via Multi-Label Classification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Disentangling Physical Dynamics From Unknown Factors for Unsupervised Video Prediction.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Reinforcement Learning of Transferable Meta-Skills for Embodied Navigation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>xMUDA: Cross-Modal Unsupervised Domain Adaptation for 3D Semantic Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Differential Treatment for Stuff and Things: A Simple Unsupervised Domain Adaptation Method for Semantic Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Modal Image Registration via Geometry Preserving Image-to-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Light-weight Calibrator: A Separable Component for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Enhanced Transport Distance for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SharinGAN: Combining Synthetic and Real Data for Unsupervised Geometry Estimation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>An Adaptive Neural Network for Unsupervised Mosaic Consistency Analysis in Image Forensics.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeFeat-Net: General Monocular Depth via Simultaneous Unsupervised Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Model Personalization While Preserving Privacy and Scalability: An Open Problem.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Invariant Representation for Unsupervised Image Restoration.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Skeleton Merger: An Unsupervised Aligned Keypoint Detector.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PAUL: Procrustean Autoencoder for Unsupervised Lifting.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DARCNN: Domain Adaptive Region-Based Convolutional Neural Network for Unsupervised Instance Segmentation in Biomedical Images.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UPFlow: Upsampling Pyramid for Unsupervised Optical Flow Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AdCo: Adversarial Contrast for Efficient Learning of Unsupervised Representations From Self-Trained Negative Adversaries.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FixBi: Bridging Domain Spaces for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>From Synthetic to Real: Unsupervised Domain Adaptation for Animal Pose Estimation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UP-DETR: Unsupervised Pre-Training for Object Detection With Transformers.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised 3D Shape Completion Through GAN Inversion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Joint Generative and Contrastive Learning for Unsupervised Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Recorrupted-to-Recorrupted: Unsupervised Deep Learning for Image Denoising.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Feature-Level Collaboration: Joint Unsupervised Learning of Optical Flow, Stereo Depth and Camera Motion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Human Pose Estimation Through Transforming Shape Templates.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Representation Learning by Tracking Patches in Video.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Discovery of the Long-Tail in Instance Segmentation Using Hierarchical Self-Supervision.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DyStaB: Unsupervised Object Segmentation via Dynamic-Static Bootstrapping.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Progressive Unsupervised Learning for Visual Object Tracking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>A Large-Scale Study on Unsupervised Spatiotemporal Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Refining Pseudo Labels With Clustering Consensus Over Generations for Unsupervised Object Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SMURF: Self-Teaching Multi-Frame Unsupervised RAFT With Full-Image Warping.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Disentanglement of Linear-Encoded Facial Semantics.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MetaCorrection: Domain-Aware Meta Loss Correction for Unsupervised Domain Adaptation in Semantic Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Cross-Domain Gradient Discrepancy Minimization for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MeGA-CDA: Memory Guided Attention for Category-Aware Unsupervised Domain Adaptive Object Detection.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of 3D Object Categories From Videos in the Wild.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Joint Noise-Tolerant Learning and Meta Camera Shift Adaptation for Unsupervised Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DG-Font: Deformable Generative Networks for Unsupervised Font Generation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Instance Level Affinity-Based Transfer for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Hyperbolic Representation Learning via Message Passing Auto-Encoders.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>EffiScene: Efficient Per-Pixel Rigidity Inference for Unsupervised Joint Learning of Optical Flow, Depth, Camera Pose and Motion Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Brain Image Synthesis With Unsupervised Multivariate Canonical CSCl4Net.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Object Detection With LIDAR Clues.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CorrNet3D: Unsupervised End-to-End Learning of Dense Correspondence for 3D Point Clouds.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Posterior Promoted GAN With Distribution Discriminator for Unsupervised Image Synthesis.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Memory-Guided Unsupervised Image-to-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Attention and Invariance for Reinforcement Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Regressive Domain Adaptation for Unsupervised Keypoint Detection.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Target-Aware Object Discovery and Association for Unsupervised Video Multi-Object Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UnsupervisedR&amp;R: Unsupervised Point Cloud Registration via Differentiable Rendering.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeepTag: An Unsupervised Deep Learning Method for Motion Tracking on Cardiac Tagging Magnetic Resonance Images.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>NeuroMorph: Unsupervised Shape Interpolation and Correspondence in One Go.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SDD-FIQA: Unsupervised Face Image Quality Assessment With Similarity Distribution Distance.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>VDSM: Unsupervised Video Disentanglement With State-Space Modeling and Deep Mixtures of Experts.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning To Relate Depth and Semantics for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Part Segmentation Through Disentangling Appearance and Shape.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rethinking Class Relations: Absolute-Relative Supervised and Unsupervised Few-Shot Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Progressive Stage-Wise Learning for Unsupervised Feature Representation Enhancement.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Source Domain Adaptation Without Access to Source Data.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Recurrent Multi-View Alignment Network for Unsupervised Surface Registration.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning for Robust Fitting: A Reinforcement Learning Approach.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ST3D: Self-Training for Unsupervised Domain Adaptation on 3D Object Detection.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Degradation Representation Learning for Blind Super-Resolution.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Smoothing the Disentangled Latent Style Space for Unsupervised Image-to-Image Translation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Clusformer: A Transformer Based Clustering Approach to Unsupervised Large-Scale Face and Visual Landmark Recognition.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Temporally-Weighted Hierarchical Clustering for Unsupervised Action Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Jigsaw Clustering for Unsupervised Visual Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Intra-Inter Camera Similarity for Unsupervised Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Improving Unsupervised Image Clustering With Robust Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PixMatch: Unsupervised Domain Adaptation via Pixelwise Consistency Training.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Hyperbolic Metric Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Feature Learning by Cross-Level Instance-Group Discrimination.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Action Shuffle Alternating Learning for Unsupervised Action Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>KeypointDeformer: Unsupervised 3D Keypoint Discovery for Shape Control.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Source Domain Adaptation for Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Real-World Image Super Resolution via Domain-Distance Aware Training.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Prototypical Cross-Domain Self-Supervised Learning for Few-Shot Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Relative Order Analysis and Optimization for Unsupervised Deep Metric Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Pre-Training for Person Re-Identification.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Dynamic Weighted Learning for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DRANet: Disentangling Representation and Adaptation Networks for Unsupervised Cross-Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reciprocal Transformations for Unsupervised Video Object Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Depth and Depth-of-Field Effect From Natural Images With Aperture Rendering Generative Adversarial Networks.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DANNet: A One-Stage Domain Adaptation Network for Unsupervised Nighttime Semantic Segmentation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Track, Check, Repeat: An EM Approach to Unsupervised Tracking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MetaAlign: Coordinating Domain Alignment and Classification for Unsupervised Domain Adaptation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Propagate Yourself: Exploring Pixel-Level Consistency for Unsupervised Visual Representation Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PiCIE: Unsupervised Semantic Segmentation Using Invariance and Equivariance in Clustering.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -933,7 +1115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716AAE81-83D8-4D04-BC65-4AB6001F7D33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606BC7CB-D096-4B10-BB7A-ABC290299CD9}">
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
small fix on junk words.
</commit_message>
<xml_diff>
--- a/example/titles.xlsx
+++ b/example/titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Programming\Python-spider-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D8413F4-1C91-427B-BEFE-206D137D8960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC9CE1B9-08CE-4269-9707-FF877A6B7B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11325" xr2:uid="{DA9FE468-2ED0-42D0-8FAA-527D3070BDF3}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11325" xr2:uid="{506579DD-23F6-44E3-A383-AFE140CD5F2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,731 +28,549 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Progressive Feature Alignment for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Open Domain Recognition by Semantic Discrepancy Minimization.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Moving Object Detection via Contextual Information Separation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Consensus Maximization for 3D Vision Problems.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Event-Based Learning of Optical Flow, Depth, and Egomotion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Tracking.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Tracking by Animation: Unsupervised Learning of Multi-Object Attentive Trackers.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Latent Filter Scaling for Multimodal Unsupervised Image-To-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Iterative Reorganization With Weak Spatial Constraints: Solving Arbitrary Jigsaw Puzzles for Unsupervised Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification by Soft Multilabel Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transferrable Prototypical Networks for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Image Generation With Semantic Parsing Transformation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Geometry-Consistent Generative Adversarial Networks for One-Sided Unsupervised Domain Mapping.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AET vs. AED: Unsupervised Representation Learning by Auto-Encoding Transformations Rather Than Data.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Towards Scene Understanding: Unsupervised Monocular Depth Estimation With Semantic-Aware Representation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DistillHash: Unsupervised Deep Hashing by Distilling Data Pairs.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Unsupervised Video Object Segmentation Through Visual Attention.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>See More, Know More: Unsupervised Video Object Segmentation With Co-Attention Siamese Networks.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Patch-Based Discriminative Feature Learning for Unsupervised Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Image Captioning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Dense Shape Correspondence.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Domain Adaptation: A Deep Max-Margin Gaussian Process Approach.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Contrastive Adaptation Network for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation for ToF Data Denoising With Adversarial Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Bilateral Cyclic Constraint and Adaptive Regularization for Unsupervised Monocular Depth Prediction.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised 3D Pose Estimation With Geometric Self-Supervision.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Embedding Learning via Invariant and Spreading Instance Feature.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Noise-Aware Unsupervised Deep Lidar-Stereo Fusion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FineGAN: Unsupervised Hierarchical Disentanglement for Fine-Grained Object Generation and Discovery.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Domain-Specific Batch Normalization for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TransGaGa: Geometry-Aware Unsupervised Image-To-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UnOS: Unified Unsupervised Optical-Flow and Stereo-Depth Estimation by Watching Videos.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GCAN: Graph Convolutional Adversarial Network for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Image Matching and Object Discovery as Optimization.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transfer Learning via Unsupervised Task Discovery for Visual Question Answering.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeepMapping: Unsupervised Map Estimation From Multiple Point Clouds.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Deep Multimodal Clustering for Unsupervised Audiovisual Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation Using Feature-Whitening and Consensus Loss.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MVTec AD - A Comprehensive Real-World Dataset for Unsupervised Anomaly Detection.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Primitive Discovery for Improved 3D Generative Modeling.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Refine and Distill: Exploiting Cycle-Inconsistency and Knowledge Distillation for Unsupervised Monocular Depth Estimation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SIGNet: Semantic Instance Aided Unsupervised 3D Geometry Perception.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Face Normalization With Extreme Pose and Expression in the Wild.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain-Specific Deblurring via Disentangled Representations.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Sliced Wasserstein Discrepancy for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Disentangling of Appearance and Geometry by Deformable Generator Network.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Modal Neural Machine Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Part-Based Disentangling of Object Shape and Appearance.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>"Double-DIP": Unsupervised Image Decomposition via Coupled Deep-Image-Priors.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Action Classes With Continuous Temporal Embedding.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Epipolar Flow for Stationary or Dynamic Scenes.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Quasi-Unsupervised Color Constancy.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Competitive Collaboration: Joint Unsupervised Learning of Depth, Camera Motion, Optical Flow and Motion Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Probably Symmetric Deformable 3D Objects From Images in the Wild.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Evolving Losses for Unsupervised Video Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Transformation GAN for Unsupervised Image Synthesis and Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Unsupervised Hierarchical Part Decomposition of 3D Objects From a Single RGB Image.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Adaptation Learning for Hyperspectral Imagery Super-Resolution.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Creating Something From Nothing: Unsupervised Knowledge Distillation for Cross-Modal Hashing.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning for Intrinsic Image Decomposition From a Single Image.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification via Softened Similarity Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Intra-Domain Adaptation for Semantic Segmentation Through Self-Supervision.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>What Can Be Transferred: Unsupervised Domain Adaptation for Endoscopic Lesions Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation With Hierarchical Gradient Synchronization.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Gum-Net: Unsupervised Geometric Matching for Fast and Accurate 3D Subtomogram Image Alignment and Averaging.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Instance Segmentation in Microscopy Images via Panoptic Domain Adaptation and Task Re-Weighting.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reliable Weighted Optimal Transport for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DUNIT: Detection-Based Unsupervised Image-to-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TransMoMo: Invariance-Driven Unsupervised Video Motion Retargeting.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Global-Local Bidirectional Reasoning for Unsupervised Representation Learning of 3D Point Clouds.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Probabilistic Structural Latent Representation for Unsupervised Embedding.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SER-FIQ: Unsupervised Estimation of Face Image Quality Based on Stochastic Embedding Robustness.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UCTGAN: Diverse Image Inpainting Based on Unsupervised Cross-Space Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Towards Unsupervised Learning of Generative Models for 3D Controllable Image Synthesis.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rotate-and-Render: Unsupervised Photorealistic Face Rotation From Single-View Images.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning by Analogy: Reliable Supervision From Transformations for Unsupervised Optical Flow Estimation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Online Deep Clustering for Unsupervised Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GraphTER: Unsupervised Learning of Graph Transformation Equivariant Representations via Auto-Encoding Node-Wise Transformations.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Representation Learning for Gaze Estimation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reusing Discriminators for Encoding: Towards Unsupervised Image-to-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Magnification of Posture Deviations Across Subjects.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Domain Adaptation via Structurally Regularized Deep Clustering.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Stochastic Classifiers for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Intrinsic Structural Representation Points.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Deep Shape Descriptor With Point Distribution Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning From Video With Deep Neural Embeddings.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PREDICT &amp; CLUSTER: Unsupervised Skeleton Based Action Recognition.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Model Adaptation: Unsupervised Domain Adaptation Without Source Data.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ProAlignNet: Unsupervised Learning for Progressively Aligning Noisy Contours.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Momentum Contrast for Unsupervised Visual Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Temporal Co-Attention Models for Unsupervised Video Action Localization.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Visual Grounding in Video for Unsupervised Word Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Person Re-Identification via Multi-Label Classification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Disentangling Physical Dynamics From Unknown Factors for Unsupervised Video Prediction.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Reinforcement Learning of Transferable Meta-Skills for Embodied Navigation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>xMUDA: Cross-Modal Unsupervised Domain Adaptation for 3D Semantic Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Differential Treatment for Stuff and Things: A Simple Unsupervised Domain Adaptation Method for Semantic Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Modal Image Registration via Geometry Preserving Image-to-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Light-weight Calibrator: A Separable Component for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Enhanced Transport Distance for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SharinGAN: Combining Synthetic and Real Data for Unsupervised Geometry Estimation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>An Adaptive Neural Network for Unsupervised Mosaic Consistency Analysis in Image Forensics.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeFeat-Net: General Monocular Depth via Simultaneous Unsupervised Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Model Personalization While Preserving Privacy and Scalability: An Open Problem.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning Invariant Representation for Unsupervised Image Restoration.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Skeleton Merger: An Unsupervised Aligned Keypoint Detector.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PAUL: Procrustean Autoencoder for Unsupervised Lifting.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DARCNN: Domain Adaptive Region-Based Convolutional Neural Network for Unsupervised Instance Segmentation in Biomedical Images.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UPFlow: Upsampling Pyramid for Unsupervised Optical Flow Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AdCo: Adversarial Contrast for Efficient Learning of Unsupervised Representations From Self-Trained Negative Adversaries.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>FixBi: Bridging Domain Spaces for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>From Synthetic to Real: Unsupervised Domain Adaptation for Animal Pose Estimation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UP-DETR: Unsupervised Pre-Training for Object Detection With Transformers.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised 3D Shape Completion Through GAN Inversion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Joint Generative and Contrastive Learning for Unsupervised Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Recorrupted-to-Recorrupted: Unsupervised Deep Learning for Image Denoising.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Feature-Level Collaboration: Joint Unsupervised Learning of Optical Flow, Stereo Depth and Camera Motion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Human Pose Estimation Through Transforming Shape Templates.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Representation Learning by Tracking Patches in Video.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Discovery of the Long-Tail in Instance Segmentation Using Hierarchical Self-Supervision.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DyStaB: Unsupervised Object Segmentation via Dynamic-Static Bootstrapping.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Progressive Unsupervised Learning for Visual Object Tracking.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>A Large-Scale Study on Unsupervised Spatiotemporal Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Refining Pseudo Labels With Clustering Consensus Over Generations for Unsupervised Object Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SMURF: Self-Teaching Multi-Frame Unsupervised RAFT With Full-Image Warping.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Disentanglement of Linear-Encoded Facial Semantics.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MetaCorrection: Domain-Aware Meta Loss Correction for Unsupervised Domain Adaptation in Semantic Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Cross-Domain Gradient Discrepancy Minimization for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MeGA-CDA: Memory Guided Attention for Category-Aware Unsupervised Domain Adaptive Object Detection.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of 3D Object Categories From Videos in the Wild.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Joint Noise-Tolerant Learning and Meta Camera Shift Adaptation for Unsupervised Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DG-Font: Deformable Generative Networks for Unsupervised Font Generation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Instance Level Affinity-Based Transfer for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Hyperbolic Representation Learning via Message Passing Auto-Encoders.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>EffiScene: Efficient Per-Pixel Rigidity Inference for Unsupervised Joint Learning of Optical Flow, Depth, Camera Pose and Motion Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Brain Image Synthesis With Unsupervised Multivariate Canonical CSCl4Net.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Object Detection With LIDAR Clues.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CorrNet3D: Unsupervised End-to-End Learning of Dense Correspondence for 3D Point Clouds.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Posterior Promoted GAN With Distribution Discriminator for Unsupervised Image Synthesis.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Memory-Guided Unsupervised Image-to-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Visual Attention and Invariance for Reinforcement Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Regressive Domain Adaptation for Unsupervised Keypoint Detection.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Target-Aware Object Discovery and Association for Unsupervised Video Multi-Object Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>UnsupervisedR&amp;R: Unsupervised Point Cloud Registration via Differentiable Rendering.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DeepTag: An Unsupervised Deep Learning Method for Motion Tracking on Cardiac Tagging Magnetic Resonance Images.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>NeuroMorph: Unsupervised Shape Interpolation and Correspondence in One Go.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SDD-FIQA: Unsupervised Face Image Quality Assessment With Similarity Distribution Distance.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>VDSM: Unsupervised Video Disentanglement With State-Space Modeling and Deep Mixtures of Experts.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Learning To Relate Depth and Semantics for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Part Segmentation Through Disentangling Appearance and Shape.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rethinking Class Relations: Absolute-Relative Supervised and Unsupervised Few-Shot Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Progressive Stage-Wise Learning for Unsupervised Feature Representation Enhancement.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Source Domain Adaptation Without Access to Source Data.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Recurrent Multi-View Alignment Network for Unsupervised Surface Registration.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning for Robust Fitting: A Reinforcement Learning Approach.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ST3D: Self-Training for Unsupervised Domain Adaptation on 3D Object Detection.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Degradation Representation Learning for Blind Super-Resolution.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Smoothing the Disentangled Latent Style Space for Unsupervised Image-to-Image Translation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Clusformer: A Transformer Based Clustering Approach to Unsupervised Large-Scale Face and Visual Landmark Recognition.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Temporally-Weighted Hierarchical Clustering for Unsupervised Action Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Jigsaw Clustering for Unsupervised Visual Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Intra-Inter Camera Similarity for Unsupervised Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Improving Unsupervised Image Clustering With Robust Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PixMatch: Unsupervised Domain Adaptation via Pixelwise Consistency Training.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Hyperbolic Metric Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Feature Learning by Cross-Level Instance-Group Discrimination.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Action Shuffle Alternating Learning for Unsupervised Action Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>KeypointDeformer: Unsupervised 3D Keypoint Discovery for Shape Control.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Multi-Source Domain Adaptation for Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Real-World Image Super Resolution via Domain-Distance Aware Training.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Prototypical Cross-Domain Self-Supervised Learning for Few-Shot Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Relative Order Analysis and Optimization for Unsupervised Deep Metric Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Pre-Training for Person Re-Identification.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Dynamic Weighted Learning for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DRANet: Disentangling Representation and Adaptation Networks for Unsupervised Cross-Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Reciprocal Transformations for Unsupervised Video Object Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Unsupervised Learning of Depth and Depth-of-Field Effect From Natural Images With Aperture Rendering Generative Adversarial Networks.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DANNet: A One-Stage Domain Adaptation Network for Unsupervised Nighttime Semantic Segmentation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Track, Check, Repeat: An EM Approach to Unsupervised Tracking.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MetaAlign: Coordinating Domain Alignment and Classification for Unsupervised Domain Adaptation.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Propagate Yourself: Exploring Pixel-Level Consistency for Unsupervised Visual Representation Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PiCIE: Unsupervised Semantic Segmentation Using Invariance and Equivariance in Clustering.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1115,7 +933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606BC7CB-D096-4B10-BB7A-ABC290299CD9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AB1A65-F9BE-42F7-815B-DCBC196FF044}">
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>